<commit_message>
bottom menu 이미지 변경 및 text color 변경
</commit_message>
<xml_diff>
--- a/Interface 문서/고객용_인터페이스설계서_V1.2_20200423.xlsx
+++ b/Interface 문서/고객용_인터페이스설계서_V1.2_20200423.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="749" firstSheet="22" activeTab="28"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="749" firstSheet="27" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="겉표지" sheetId="2" r:id="rId1"/>
@@ -3290,7 +3290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3668" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3684" uniqueCount="802">
   <si>
     <t>버전</t>
   </si>
@@ -4982,10 +4982,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>REGISTER_RECOM_CODE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MY_POINT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5086,10 +5082,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">17~18, 19~20, 21~24 반복 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> {"coupone_list": [{"TOTAL":"5","CURRENT_PAGE":"1","CURRENT_NUM":"20"}],"data":[{"COUPONE_SEQ":"1","COUPONE_PAY":"2000","COUPONE_TITLE":"추천인 할인 쿠폰","COUPONE_CONTENT":"회원 가입을 축하해요!","COUPONE_DATE":"~2019.12.31","COUPONE_YN":"N"},{},{}…]}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5231,10 +5223,6 @@
   </si>
   <si>
     <t>NICKNAME</t>
-    <phoneticPr fontId="34" type="noConversion"/>
-  </si>
-  <si>
-    <t>RECOMMAND</t>
     <phoneticPr fontId="34" type="noConversion"/>
   </si>
   <si>
@@ -5944,11 +5932,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>http://~~~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원타입(0:일반회원, 1:매니져)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WASH_AREA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세차 가능 지역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관악구,금천구,영등포구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추천인 코드 (휴대폰번호)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01012345678</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01012345678</t>
+    <phoneticPr fontId="34" type="noConversion"/>
+  </si>
+  <si>
+    <t>RECOMMAND</t>
+    <phoneticPr fontId="34" type="noConversion"/>
+  </si>
+  <si>
+    <t>REGISTER_RECOM_CODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGENT_IMG_URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>대리점  담당자 프로필 이미지 URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://~~~</t>
+    <t>CAR_TYPE</t>
+    <phoneticPr fontId="34" type="noConversion"/>
+  </si>
+  <si>
+    <t>차량 타입</t>
+    <phoneticPr fontId="34" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAR_TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차량 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">17~18, 19~20, 21~25 반복 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -5956,36 +6008,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원타입(0:일반회원, 1:매니져)</t>
+    <t>CAR_TYPE</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AGENT_IMG_URL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WASH_AREA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>세차 가능 지역</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관악구,금천구,영등포구</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추천인 코드 (휴대폰번호)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01012345678</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>01012345678</t>
-    <phoneticPr fontId="34" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6376,7 +6400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -6935,6 +6959,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -6950,7 +6987,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="272">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -7721,6 +7758,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal 2" xfId="5"/>
@@ -8474,7 +8517,7 @@
   </sheetPr>
   <dimension ref="B1:O68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -8887,7 +8930,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -9010,10 +9053,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="E24" s="62">
         <v>21352</v>
@@ -9054,13 +9097,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D25" s="62" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="E25" s="118" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="F25" s="62" t="s">
         <v>232</v>
@@ -10562,7 +10605,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -10650,7 +10693,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>291</v>
@@ -10694,7 +10737,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>246</v>
@@ -15333,7 +15376,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -15456,7 +15499,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -15544,7 +15587,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>291</v>
@@ -16590,7 +16633,9 @@
   </sheetPr>
   <dimension ref="B1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J27" sqref="J27:O27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16999,7 +17044,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -17143,7 +17188,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="K24" s="62" t="s">
         <v>234</v>
@@ -17187,7 +17232,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K25" s="62" t="s">
         <v>276</v>
@@ -17231,10 +17276,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="127" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K26" s="62" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L26" s="62">
         <v>50000</v>
@@ -17274,22 +17319,34 @@
       <c r="I27" s="61">
         <v>4</v>
       </c>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="64"/>
+      <c r="J27" s="272" t="s">
+        <v>801</v>
+      </c>
+      <c r="K27" s="180" t="s">
+        <v>798</v>
+      </c>
+      <c r="L27" s="180">
+        <v>1</v>
+      </c>
+      <c r="M27" s="180" t="s">
+        <v>232</v>
+      </c>
+      <c r="N27" s="180">
+        <v>3</v>
+      </c>
+      <c r="O27" s="182" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="28" spans="2:15" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="57">
         <v>5</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="E28" s="62">
         <v>11</v>
@@ -17318,10 +17375,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="E29" s="62">
         <v>11</v>
@@ -18203,7 +18260,7 @@
   <dimension ref="B1:O68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -18613,7 +18670,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -18736,7 +18793,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -18824,7 +18881,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>291</v>
@@ -19049,10 +19106,10 @@
         <v>9</v>
       </c>
       <c r="J32" s="110" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K32" s="62" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L32" s="62">
         <v>50000</v>
@@ -19080,12 +19137,24 @@
       <c r="I33" s="61">
         <v>10</v>
       </c>
-      <c r="J33" s="110"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="64"/>
+      <c r="J33" s="272" t="s">
+        <v>801</v>
+      </c>
+      <c r="K33" s="180" t="s">
+        <v>798</v>
+      </c>
+      <c r="L33" s="180">
+        <v>1</v>
+      </c>
+      <c r="M33" s="180" t="s">
+        <v>232</v>
+      </c>
+      <c r="N33" s="180">
+        <v>3</v>
+      </c>
+      <c r="O33" s="182" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="34" spans="2:15" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="57">
@@ -19864,7 +19933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -20275,7 +20344,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -20398,10 +20467,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E24" s="98">
         <v>1098761234</v>
@@ -20442,10 +20511,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
+        <v>555</v>
+      </c>
+      <c r="D25" s="58" t="s">
         <v>556</v>
-      </c>
-      <c r="D25" s="58" t="s">
-        <v>557</v>
       </c>
       <c r="E25" s="62">
         <v>21352</v>
@@ -20484,10 +20553,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E26" s="58">
         <v>1</v>
@@ -20516,10 +20585,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
+        <v>552</v>
+      </c>
+      <c r="D27" s="58" t="s">
         <v>553</v>
-      </c>
-      <c r="D27" s="58" t="s">
-        <v>554</v>
       </c>
       <c r="E27" s="98" t="s">
         <v>328</v>
@@ -21440,7 +21509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:H27"/>
     </sheetView>
   </sheetViews>
@@ -21848,7 +21917,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -21971,7 +22040,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -22059,7 +22128,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>291</v>
@@ -22103,7 +22172,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>246</v>
@@ -22156,13 +22225,13 @@
         <v>5</v>
       </c>
       <c r="J28" s="110" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="K28" s="62" t="s">
         <v>430</v>
       </c>
       <c r="L28" s="58" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="M28" s="62" t="s">
         <v>232</v>
@@ -22188,13 +22257,13 @@
         <v>6</v>
       </c>
       <c r="J29" s="110" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="K29" s="62" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="L29" s="62" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="M29" s="62" t="s">
         <v>232</v>
@@ -23473,7 +23542,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -23596,10 +23665,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="E24" s="62">
         <v>2.13522020040112E+18</v>
@@ -23684,13 +23753,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="F26" s="62" t="s">
         <v>232</v>
@@ -23705,10 +23774,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K26" s="62" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L26" s="108">
         <v>35670</v>
@@ -23728,10 +23797,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E27" s="58">
         <v>2020</v>
@@ -23760,10 +23829,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E28" s="58">
         <v>10</v>
@@ -23792,10 +23861,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E29" s="58">
         <v>30</v>
@@ -23827,7 +23896,7 @@
         <v>528</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E30" s="58">
         <v>1</v>
@@ -23856,10 +23925,10 @@
         <v>8</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E31" s="62" t="s">
         <v>354</v>
@@ -23888,10 +23957,10 @@
         <v>9</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E32" s="129">
         <v>0.45833333333333331</v>
@@ -23920,7 +23989,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D33" s="58" t="s">
         <v>434</v>
@@ -23952,13 +24021,13 @@
         <v>11</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D34" s="58" t="s">
         <v>435</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F34" s="62" t="s">
         <v>232</v>
@@ -23982,7 +24051,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D35" s="58" t="s">
         <v>431</v>
@@ -24014,7 +24083,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D36" s="58" t="s">
         <v>432</v>
@@ -24046,7 +24115,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D37" s="58" t="s">
         <v>433</v>
@@ -24078,7 +24147,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D38" s="58" t="s">
         <v>460</v>
@@ -24110,7 +24179,7 @@
         <v>16</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D39" s="58" t="s">
         <v>436</v>
@@ -24140,7 +24209,7 @@
         <v>17</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D40" s="58" t="s">
         <v>437</v>
@@ -24907,13 +24976,13 @@
     <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="20" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>144</v>
@@ -24923,13 +24992,13 @@
     <row r="8" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20"/>
       <c r="B8" s="20" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C8" s="21">
         <v>43920</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>144</v>
@@ -30195,7 +30264,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -30362,7 +30431,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>251</v>
@@ -31746,7 +31815,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -31890,7 +31959,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="K24" s="62" t="s">
         <v>334</v>
@@ -32622,7 +32691,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -32907,7 +32976,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -33030,7 +33099,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -33118,7 +33187,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>291</v>
@@ -33162,7 +33231,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>246</v>
@@ -33215,10 +33284,10 @@
         <v>5</v>
       </c>
       <c r="J28" s="110" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="K28" s="62" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="L28" s="62" t="s">
         <v>338</v>
@@ -33247,7 +33316,7 @@
         <v>6</v>
       </c>
       <c r="J29" s="110" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="K29" s="62" t="s">
         <v>335</v>
@@ -33279,7 +33348,7 @@
         <v>7</v>
       </c>
       <c r="J30" s="110" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="K30" s="62" t="s">
         <v>336</v>
@@ -33311,7 +33380,7 @@
         <v>8</v>
       </c>
       <c r="J31" s="110" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="K31" s="62" t="s">
         <v>337</v>
@@ -33766,8 +33835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -34172,7 +34241,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -34316,10 +34385,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="122" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K24" s="62" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="L24" s="62">
         <v>1</v>
@@ -34360,10 +34429,10 @@
         <v>2</v>
       </c>
       <c r="J25" s="122" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="K25" s="62" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="L25" s="58" t="s">
         <v>419</v>
@@ -34392,13 +34461,13 @@
         <v>3</v>
       </c>
       <c r="J26" s="122" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="K26" s="62" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="L26" s="58" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="M26" s="62" t="s">
         <v>232</v>
@@ -34424,13 +34493,13 @@
         <v>4</v>
       </c>
       <c r="J27" s="122" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="K27" s="62" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="L27" s="58" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="M27" s="62" t="s">
         <v>232</v>
@@ -34456,10 +34525,10 @@
         <v>5</v>
       </c>
       <c r="J28" s="122" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="K28" s="62" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="L28" s="62">
         <v>50000</v>
@@ -34487,22 +34556,22 @@
       <c r="I29" s="61">
         <v>6</v>
       </c>
-      <c r="J29" s="110" t="s">
-        <v>305</v>
-      </c>
-      <c r="K29" s="62" t="s">
-        <v>292</v>
-      </c>
-      <c r="L29" s="62">
-        <v>20</v>
-      </c>
-      <c r="M29" s="62" t="s">
+      <c r="J29" s="272" t="s">
+        <v>795</v>
+      </c>
+      <c r="K29" s="180" t="s">
+        <v>796</v>
+      </c>
+      <c r="L29" s="180">
+        <v>1</v>
+      </c>
+      <c r="M29" s="180" t="s">
         <v>232</v>
       </c>
-      <c r="N29" s="63">
-        <v>10</v>
-      </c>
-      <c r="O29" s="64" t="s">
+      <c r="N29" s="180">
+        <v>3</v>
+      </c>
+      <c r="O29" s="182" t="s">
         <v>140</v>
       </c>
     </row>
@@ -34520,19 +34589,19 @@
         <v>7</v>
       </c>
       <c r="J30" s="110" t="s">
-        <v>530</v>
+        <v>305</v>
       </c>
       <c r="K30" s="62" t="s">
-        <v>493</v>
+        <v>292</v>
       </c>
       <c r="L30" s="62">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="M30" s="62" t="s">
         <v>232</v>
       </c>
       <c r="N30" s="63">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O30" s="64" t="s">
         <v>140</v>
@@ -34552,19 +34621,19 @@
         <v>8</v>
       </c>
       <c r="J31" s="110" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="K31" s="62" t="s">
-        <v>526</v>
+        <v>493</v>
       </c>
       <c r="L31" s="62">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="M31" s="62" t="s">
         <v>232</v>
       </c>
       <c r="N31" s="63">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O31" s="64" t="s">
         <v>140</v>
@@ -34584,19 +34653,19 @@
         <v>9</v>
       </c>
       <c r="J32" s="110" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="K32" s="62" t="s">
-        <v>494</v>
+        <v>526</v>
       </c>
       <c r="L32" s="62">
-        <v>2000</v>
+        <v>20</v>
       </c>
       <c r="M32" s="62" t="s">
         <v>232</v>
       </c>
       <c r="N32" s="63">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O32" s="64" t="s">
         <v>140</v>
@@ -34615,14 +34684,24 @@
       <c r="I33" s="61">
         <v>10</v>
       </c>
-      <c r="J33" s="62"/>
+      <c r="J33" s="110" t="s">
+        <v>531</v>
+      </c>
       <c r="K33" s="62" t="s">
-        <v>495</v>
-      </c>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="64"/>
+        <v>494</v>
+      </c>
+      <c r="L33" s="62">
+        <v>2000</v>
+      </c>
+      <c r="M33" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="N33" s="63">
+        <v>10</v>
+      </c>
+      <c r="O33" s="64" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="34" spans="2:15" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="57">
@@ -34638,7 +34717,9 @@
         <v>11</v>
       </c>
       <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
+      <c r="K34" s="62" t="s">
+        <v>495</v>
+      </c>
       <c r="L34" s="62"/>
       <c r="M34" s="62"/>
       <c r="N34" s="63"/>
@@ -35427,7 +35508,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -35594,7 +35675,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>505</v>
@@ -35638,7 +35719,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>291</v>
@@ -35659,13 +35740,13 @@
         <v>3</v>
       </c>
       <c r="J26" s="110" t="s">
+        <v>681</v>
+      </c>
+      <c r="K26" s="62" t="s">
+        <v>682</v>
+      </c>
+      <c r="L26" s="62" t="s">
         <v>684</v>
-      </c>
-      <c r="K26" s="62" t="s">
-        <v>685</v>
-      </c>
-      <c r="L26" s="62" t="s">
-        <v>687</v>
       </c>
       <c r="M26" s="62" t="s">
         <v>287</v>
@@ -35682,7 +35763,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>246</v>
@@ -35706,10 +35787,10 @@
         <v>507</v>
       </c>
       <c r="K27" s="62" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="L27" s="62" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="M27" s="62" t="s">
         <v>232</v>
@@ -36240,9 +36321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -36263,7 +36342,7 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="96" t="s">
-        <v>235</v>
+        <v>792</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="40"/>
@@ -36361,7 +36440,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -36474,7 +36553,7 @@
       </c>
       <c r="C11" s="215"/>
       <c r="D11" s="255" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="E11" s="217"/>
       <c r="F11" s="217"/>
@@ -36646,7 +36725,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -36813,7 +36892,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>508</v>
@@ -36834,7 +36913,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="K25" s="62" t="s">
         <v>299</v>
@@ -36857,7 +36936,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>534</v>
@@ -36878,7 +36957,7 @@
         <v>3</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="K26" s="62" t="s">
         <v>300</v>
@@ -36901,7 +36980,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D27" s="58" t="s">
         <v>291</v>
@@ -36945,7 +37024,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D28" s="58" t="s">
         <v>246</v>
@@ -36966,10 +37045,10 @@
         <v>5</v>
       </c>
       <c r="J28" s="110" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="K28" s="62" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="L28" s="62" t="s">
         <v>509</v>
@@ -36989,7 +37068,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="177" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="D29" s="177" t="s">
         <v>505</v>
@@ -37042,13 +37121,13 @@
         <v>7</v>
       </c>
       <c r="J30" s="179" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="K30" s="180" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="L30" s="181" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="M30" s="180" t="s">
         <v>232</v>
@@ -37074,13 +37153,13 @@
         <v>8</v>
       </c>
       <c r="J31" s="168" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="K31" s="169" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="L31" s="169" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="M31" s="169" t="s">
         <v>232</v>
@@ -37106,13 +37185,13 @@
         <v>9</v>
       </c>
       <c r="J32" s="168" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="K32" s="169" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="L32" s="169" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="M32" s="169" t="s">
         <v>232</v>
@@ -37138,10 +37217,10 @@
         <v>10</v>
       </c>
       <c r="J33" s="168" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="K33" s="169" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="L33" s="169">
         <v>1</v>
@@ -37173,7 +37252,7 @@
         <v>524</v>
       </c>
       <c r="K34" s="62" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="L34" s="118" t="s">
         <v>535</v>
@@ -37202,10 +37281,10 @@
         <v>12</v>
       </c>
       <c r="J35" s="110" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="K35" s="62" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="L35" s="62" t="s">
         <v>536</v>
@@ -37578,8 +37657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -37699,7 +37778,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -37984,7 +38063,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -38107,7 +38186,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -38128,10 +38207,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="K24" s="100" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="L24" s="62" t="s">
         <v>270</v>
@@ -38151,13 +38230,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F25" s="58" t="s">
         <v>232</v>
@@ -38172,7 +38251,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="K25" s="101" t="s">
         <v>272</v>
@@ -38193,13 +38272,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="F26" s="58" t="s">
         <v>232</v>
@@ -38225,13 +38304,13 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>608</v>
+        <v>790</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E27" s="98" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="F27" s="58" t="s">
         <v>232</v>
@@ -38257,13 +38336,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F28" s="58" t="s">
         <v>232</v>
@@ -38289,13 +38368,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="58" t="s">
+        <v>614</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>612</v>
+      </c>
+      <c r="E29" s="58" t="s">
         <v>617</v>
-      </c>
-      <c r="D29" s="58" t="s">
-        <v>615</v>
-      </c>
-      <c r="E29" s="58" t="s">
-        <v>620</v>
       </c>
       <c r="F29" s="58" t="s">
         <v>232</v>
@@ -38321,13 +38400,13 @@
         <v>7</v>
       </c>
       <c r="C30" s="58" t="s">
+        <v>615</v>
+      </c>
+      <c r="D30" s="58" t="s">
         <v>618</v>
       </c>
-      <c r="D30" s="58" t="s">
-        <v>621</v>
-      </c>
       <c r="E30" s="58" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F30" s="58" t="s">
         <v>232</v>
@@ -38353,13 +38432,13 @@
         <v>8</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F31" s="58" t="s">
         <v>232</v>
@@ -38816,8 +38895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -38882,7 +38961,7 @@
         <v>252</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="36"/>
@@ -38901,10 +38980,10 @@
         <v>261</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -38923,10 +39002,10 @@
         <v>263</v>
       </c>
       <c r="C6" s="142" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D6" s="143" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E6" s="142"/>
       <c r="F6" s="142"/>
@@ -38945,7 +39024,7 @@
         <v>264</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D7" s="37" t="s">
         <v>265</v>
@@ -38967,10 +39046,10 @@
         <v>281</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
@@ -38992,7 +39071,7 @@
         <v>357</v>
       </c>
       <c r="D9" s="91" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
@@ -39014,7 +39093,7 @@
         <v>367</v>
       </c>
       <c r="D10" s="91" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="91"/>
@@ -39036,7 +39115,7 @@
         <v>369</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="91"/>
@@ -39058,7 +39137,7 @@
         <v>383</v>
       </c>
       <c r="D12" s="146" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="E12" s="142"/>
       <c r="F12" s="146"/>
@@ -39080,7 +39159,7 @@
         <v>382</v>
       </c>
       <c r="D13" s="146" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E13" s="142"/>
       <c r="F13" s="146"/>
@@ -39149,7 +39228,7 @@
         <v>422</v>
       </c>
       <c r="D16" s="91" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="91"/>
@@ -39193,7 +39272,7 @@
         <v>424</v>
       </c>
       <c r="D18" s="148" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E18" s="149"/>
       <c r="F18" s="148"/>
@@ -39237,7 +39316,7 @@
         <v>438</v>
       </c>
       <c r="D20" s="148" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="E20" s="149"/>
       <c r="F20" s="148"/>
@@ -39259,7 +39338,7 @@
         <v>439</v>
       </c>
       <c r="D21" s="148" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="E21" s="149"/>
       <c r="F21" s="148"/>
@@ -39281,7 +39360,7 @@
         <v>440</v>
       </c>
       <c r="D22" s="146" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="E22" s="142"/>
       <c r="F22" s="146"/>
@@ -39341,7 +39420,7 @@
     </row>
     <row r="25" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="120" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C25" s="91" t="s">
         <v>465</v>
@@ -39363,13 +39442,13 @@
     </row>
     <row r="26" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="128" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C26" s="91" t="s">
+        <v>560</v>
+      </c>
+      <c r="D26" s="91" t="s">
         <v>561</v>
-      </c>
-      <c r="D26" s="91" t="s">
-        <v>562</v>
       </c>
       <c r="E26" s="91"/>
       <c r="F26" s="91"/>
@@ -39385,7 +39464,7 @@
     </row>
     <row r="27" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="120" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C27" s="91" t="s">
         <v>502</v>
@@ -39407,7 +39486,7 @@
     </row>
     <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="120" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C28" s="91" t="s">
         <v>510</v>
@@ -39429,13 +39508,13 @@
     </row>
     <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="120" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C29" s="91" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D29" s="91" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E29" s="91"/>
       <c r="F29" s="91"/>
@@ -39451,13 +39530,13 @@
     </row>
     <row r="30" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="120" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C30" s="91" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D30" s="91" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="E30" s="91"/>
       <c r="F30" s="91"/>
@@ -39473,13 +39552,13 @@
     </row>
     <row r="31" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="120" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C31" s="91" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="D31" s="91" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="E31" s="91"/>
       <c r="F31" s="91"/>
@@ -39495,13 +39574,13 @@
     </row>
     <row r="32" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="120" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="C32" s="91" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D32" s="91" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="E32" s="91"/>
       <c r="F32" s="91"/>
@@ -39517,13 +39596,13 @@
     </row>
     <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="120" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="C33" s="91" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D33" s="91" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="E33" s="91"/>
       <c r="F33" s="91"/>
@@ -39670,7 +39749,7 @@
   <dimension ref="B1:O48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -39793,7 +39872,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -39998,7 +40077,7 @@
       </c>
       <c r="C15" s="229"/>
       <c r="D15" s="216" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="E15" s="217"/>
       <c r="F15" s="217"/>
@@ -40080,7 +40159,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -40203,10 +40282,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E24" s="62">
         <v>21352</v>
@@ -40224,7 +40303,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="K24" s="62" t="s">
         <v>234</v>
@@ -40247,10 +40326,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="E25" s="58">
         <v>11</v>
@@ -40945,7 +41024,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -41150,7 +41229,7 @@
       </c>
       <c r="C15" s="229"/>
       <c r="D15" s="216" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E15" s="217"/>
       <c r="F15" s="217"/>
@@ -41232,7 +41311,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -41355,10 +41434,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="E24" s="62">
         <v>21352</v>
@@ -41376,13 +41455,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
+        <v>731</v>
+      </c>
+      <c r="K24" s="62" t="s">
         <v>734</v>
       </c>
-      <c r="K24" s="62" t="s">
-        <v>737</v>
-      </c>
       <c r="L24" s="62" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="M24" s="62" t="s">
         <v>232</v>
@@ -41399,10 +41478,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E25" s="58">
         <v>50000</v>
@@ -41420,7 +41499,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="K25" s="62" t="s">
         <v>276</v>
@@ -41441,10 +41520,10 @@
         <v>3</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D26" s="62" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="E26" s="62">
         <v>2.13522020040113E+18</v>
@@ -41462,10 +41541,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K26" s="62" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L26" s="108">
         <v>35670</v>
@@ -42121,7 +42200,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -42408,7 +42487,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -42531,7 +42610,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -42552,13 +42631,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="K24" s="100" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="L24" s="62" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="M24" s="62" t="s">
         <v>232</v>
@@ -42584,13 +42663,13 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="K25" s="101" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="L25" s="62" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="M25" s="62" t="s">
         <v>232</v>
@@ -43274,7 +43353,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -43479,7 +43558,7 @@
       </c>
       <c r="C15" s="229"/>
       <c r="D15" s="216" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E15" s="217"/>
       <c r="F15" s="217"/>
@@ -43561,7 +43640,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -43684,10 +43763,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="E24" s="62">
         <v>2.13522020040112E+18</v>
@@ -43705,13 +43784,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
+        <v>731</v>
+      </c>
+      <c r="K24" s="62" t="s">
         <v>734</v>
       </c>
-      <c r="K24" s="62" t="s">
-        <v>737</v>
-      </c>
       <c r="L24" s="62" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="M24" s="62" t="s">
         <v>232</v>
@@ -43749,7 +43828,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="K25" s="62" t="s">
         <v>276</v>
@@ -43770,13 +43849,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="F26" s="62" t="s">
         <v>232</v>
@@ -43791,10 +43870,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="K26" s="62" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L26" s="108">
         <v>35670</v>
@@ -43814,10 +43893,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E27" s="58">
         <v>2020</v>
@@ -43846,10 +43925,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E28" s="58">
         <v>10</v>
@@ -43878,10 +43957,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E29" s="58">
         <v>30</v>
@@ -43913,7 +43992,7 @@
         <v>528</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E30" s="58">
         <v>1</v>
@@ -43942,10 +44021,10 @@
         <v>8</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E31" s="62" t="s">
         <v>354</v>
@@ -43974,10 +44053,10 @@
         <v>9</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E32" s="129">
         <v>0.45833333333333331</v>
@@ -44006,7 +44085,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D33" s="58" t="s">
         <v>434</v>
@@ -44038,13 +44117,13 @@
         <v>11</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D34" s="58" t="s">
         <v>435</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F34" s="62" t="s">
         <v>232</v>
@@ -44068,7 +44147,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D35" s="58" t="s">
         <v>431</v>
@@ -44100,7 +44179,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D36" s="58" t="s">
         <v>432</v>
@@ -44132,7 +44211,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D37" s="58" t="s">
         <v>433</v>
@@ -44164,7 +44243,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D38" s="58" t="s">
         <v>460</v>
@@ -44196,7 +44275,7 @@
         <v>16</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D39" s="58" t="s">
         <v>436</v>
@@ -44226,7 +44305,7 @@
         <v>17</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D40" s="58" t="s">
         <v>437</v>
@@ -44261,7 +44340,7 @@
         <v>305</v>
       </c>
       <c r="D41" s="62" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="E41" s="62">
         <v>20</v>
@@ -44502,8 +44581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -44626,7 +44705,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -44831,7 +44910,7 @@
       </c>
       <c r="C15" s="229"/>
       <c r="D15" s="216" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="E15" s="217"/>
       <c r="F15" s="217"/>
@@ -44913,7 +44992,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -45036,10 +45115,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="E24" s="62">
         <v>2.13522020040112E+18</v>
@@ -45057,13 +45136,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
+        <v>731</v>
+      </c>
+      <c r="K24" s="62" t="s">
         <v>734</v>
       </c>
-      <c r="K24" s="62" t="s">
-        <v>737</v>
-      </c>
       <c r="L24" s="62" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="M24" s="62" t="s">
         <v>232</v>
@@ -45101,7 +45180,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="K25" s="62" t="s">
         <v>276</v>
@@ -45122,13 +45201,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="F26" s="62" t="s">
         <v>232</v>
@@ -45143,10 +45222,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="62" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K26" s="62" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L26" s="108">
         <v>35670</v>
@@ -45166,10 +45245,10 @@
         <v>4</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E27" s="58">
         <v>2020</v>
@@ -45198,10 +45277,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E28" s="58">
         <v>10</v>
@@ -45230,10 +45309,10 @@
         <v>6</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E29" s="58">
         <v>30</v>
@@ -45265,7 +45344,7 @@
         <v>528</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E30" s="58">
         <v>1</v>
@@ -45294,10 +45373,10 @@
         <v>8</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E31" s="62" t="s">
         <v>354</v>
@@ -45326,10 +45405,10 @@
         <v>9</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E32" s="129">
         <v>0.45833333333333331</v>
@@ -45358,7 +45437,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D33" s="58" t="s">
         <v>434</v>
@@ -45390,13 +45469,13 @@
         <v>11</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D34" s="58" t="s">
         <v>435</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F34" s="62" t="s">
         <v>232</v>
@@ -45420,7 +45499,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D35" s="58" t="s">
         <v>431</v>
@@ -45452,7 +45531,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D36" s="58" t="s">
         <v>432</v>
@@ -45484,7 +45563,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D37" s="58" t="s">
         <v>433</v>
@@ -45516,7 +45595,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D38" s="58" t="s">
         <v>460</v>
@@ -45548,7 +45627,7 @@
         <v>16</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D39" s="58" t="s">
         <v>436</v>
@@ -45578,7 +45657,7 @@
         <v>17</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D40" s="58" t="s">
         <v>437</v>
@@ -45613,7 +45692,7 @@
         <v>305</v>
       </c>
       <c r="D41" s="62" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="E41" s="62">
         <v>20</v>
@@ -48021,10 +48100,10 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B1:O49"/>
+  <dimension ref="B1:O50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -48432,7 +48511,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -48555,7 +48634,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -48576,7 +48655,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="K24" s="62" t="s">
         <v>280</v>
@@ -48599,7 +48678,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>243</v>
@@ -48814,7 +48893,7 @@
         <v>287</v>
       </c>
       <c r="N31" s="63">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O31" s="64"/>
     </row>
@@ -48832,7 +48911,7 @@
         <v>9</v>
       </c>
       <c r="J32" s="62" t="s">
-        <v>545</v>
+        <v>791</v>
       </c>
       <c r="K32" s="62" t="s">
         <v>544</v>
@@ -48844,7 +48923,7 @@
         <v>287</v>
       </c>
       <c r="N32" s="63">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O32" s="64"/>
     </row>
@@ -48865,7 +48944,7 @@
         <v>315</v>
       </c>
       <c r="K33" s="130" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L33" s="131" t="s">
         <v>317</v>
@@ -48952,10 +49031,10 @@
         <v>13</v>
       </c>
       <c r="J36" s="62" t="s">
+        <v>545</v>
+      </c>
+      <c r="K36" s="62" t="s">
         <v>546</v>
-      </c>
-      <c r="K36" s="62" t="s">
-        <v>547</v>
       </c>
       <c r="L36" s="108">
         <v>35670</v>
@@ -48982,10 +49061,10 @@
         <v>14</v>
       </c>
       <c r="J37" s="62" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K37" s="62" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="L37" s="62">
         <v>7</v>
@@ -49012,10 +49091,10 @@
         <v>15</v>
       </c>
       <c r="J38" s="62" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="K38" s="62" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="L38" s="62">
         <v>7</v>
@@ -49042,7 +49121,7 @@
         <v>16</v>
       </c>
       <c r="J39" s="62" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K39" s="62" t="s">
         <v>334</v>
@@ -49072,10 +49151,10 @@
         <v>17</v>
       </c>
       <c r="J40" s="180" t="s">
-        <v>787</v>
+        <v>800</v>
       </c>
       <c r="K40" s="180" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="L40" s="180">
         <v>1</v>
@@ -49162,7 +49241,7 @@
         <v>20</v>
       </c>
       <c r="J43" s="110" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K43" s="62" t="s">
         <v>497</v>
@@ -49226,7 +49305,7 @@
         <v>22</v>
       </c>
       <c r="J45" s="110" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K45" s="62" t="s">
         <v>497</v>
@@ -49322,10 +49401,10 @@
         <v>25</v>
       </c>
       <c r="J48" s="110" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="K48" s="62" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L48" s="62">
         <v>50000</v>
@@ -49340,27 +49419,59 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="2:15" s="51" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="117">
+    <row r="49" spans="2:15" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="273">
         <v>26</v>
       </c>
-      <c r="C49" s="67"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="69">
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="61">
         <v>26</v>
       </c>
-      <c r="J49" s="67"/>
-      <c r="K49" s="67" t="s">
-        <v>571</v>
-      </c>
-      <c r="L49" s="67"/>
-      <c r="M49" s="67"/>
-      <c r="N49" s="67"/>
-      <c r="O49" s="70"/>
+      <c r="J49" s="179" t="s">
+        <v>797</v>
+      </c>
+      <c r="K49" s="180" t="s">
+        <v>798</v>
+      </c>
+      <c r="L49" s="180">
+        <v>1</v>
+      </c>
+      <c r="M49" s="180" t="s">
+        <v>232</v>
+      </c>
+      <c r="N49" s="180">
+        <v>3</v>
+      </c>
+      <c r="O49" s="182" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" s="51" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="117">
+        <v>27</v>
+      </c>
+      <c r="C50" s="67"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="68"/>
+      <c r="I50" s="69">
+        <v>27</v>
+      </c>
+      <c r="J50" s="67"/>
+      <c r="K50" s="67" t="s">
+        <v>799</v>
+      </c>
+      <c r="L50" s="67"/>
+      <c r="M50" s="67"/>
+      <c r="N50" s="67"/>
+      <c r="O50" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="60">
@@ -49573,7 +49684,7 @@
       </c>
       <c r="C6" s="244"/>
       <c r="D6" s="245" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="E6" s="246"/>
       <c r="F6" s="246"/>
@@ -49860,7 +49971,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -49983,7 +50094,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>251</v>
@@ -50004,7 +50115,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="K24" s="100" t="s">
         <v>269</v>
@@ -50036,7 +50147,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="62" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="K25" s="101" t="s">
         <v>272</v>
@@ -50068,10 +50179,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="122" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="K26" s="62" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L26" s="62">
         <v>123456</v>
@@ -52166,7 +52277,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -52289,10 +52400,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="101" t="s">
+        <v>625</v>
+      </c>
+      <c r="D24" s="58" t="s">
         <v>628</v>
-      </c>
-      <c r="D24" s="58" t="s">
-        <v>631</v>
       </c>
       <c r="E24" s="58" t="s">
         <v>244</v>
@@ -52310,7 +52421,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="K24" s="62" t="s">
         <v>234</v>
@@ -52333,7 +52444,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>251</v>
@@ -52910,8 +53021,8 @@
   </sheetPr>
   <dimension ref="B1:O48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -53323,7 +53434,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -53444,7 +53555,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D24" s="62" t="s">
         <v>332</v>
@@ -53465,7 +53576,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="62" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K24" s="62" t="s">
         <v>247</v>
@@ -53488,7 +53599,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D25" s="58" t="s">
         <v>291</v>
@@ -53532,7 +53643,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D26" s="58" t="s">
         <v>246</v>
@@ -53588,7 +53699,7 @@
         <v>305</v>
       </c>
       <c r="K27" s="62" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="L27" s="62">
         <v>20</v>
@@ -53617,10 +53728,10 @@
         <v>5</v>
       </c>
       <c r="J28" s="164" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="K28" s="165" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="L28" s="166">
         <v>0</v>
@@ -53719,7 +53830,7 @@
         <v>470</v>
       </c>
       <c r="L31" s="62" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="M31" s="62" t="s">
         <v>232</v>
@@ -53841,7 +53952,7 @@
         <v>12</v>
       </c>
       <c r="J35" s="110" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="K35" s="62" t="s">
         <v>473</v>
@@ -54033,10 +54144,10 @@
         <v>18</v>
       </c>
       <c r="J41" s="168" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="K41" s="169" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="L41" s="170">
         <v>2000</v>
@@ -54065,7 +54176,7 @@
         <v>19</v>
       </c>
       <c r="J42" s="176" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K42" s="176" t="s">
         <v>436</v>
@@ -54098,7 +54209,7 @@
         <v>528</v>
       </c>
       <c r="K43" s="176" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L43" s="176">
         <v>1</v>
@@ -54127,13 +54238,13 @@
         <v>21</v>
       </c>
       <c r="J44" s="176" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="K44" s="176" t="s">
         <v>435</v>
       </c>
       <c r="L44" s="176" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="M44" s="166" t="s">
         <v>232</v>
@@ -54157,7 +54268,7 @@
         <v>22</v>
       </c>
       <c r="J45" s="176" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="K45" s="176" t="s">
         <v>431</v>
@@ -54189,7 +54300,7 @@
         <v>23</v>
       </c>
       <c r="J46" s="176" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="K46" s="176" t="s">
         <v>434</v>
@@ -54222,7 +54333,7 @@
       </c>
       <c r="J47" s="62"/>
       <c r="K47" s="62" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="L47" s="62"/>
       <c r="M47" s="62"/>
@@ -54738,7 +54849,7 @@
       </c>
       <c r="C19" s="210"/>
       <c r="D19" s="211" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E19" s="212"/>
       <c r="F19" s="212"/>
@@ -54861,7 +54972,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D24" s="62" t="s">
         <v>292</v>

</xml_diff>